<commit_message>
Changes and original uploads
Changed minor things in findprimes.c and findprimes_2.c; updated MPI_results; initial uploads of findprimes_4.c, findprimes_8.c, and findprimes_16.c
findprimes, findprimes_2, findprimes_4, and findprimes_8  finished.
</commit_message>
<xml_diff>
--- a/MPI_results.xlsx
+++ b/MPI_results.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10353" windowHeight="4047"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10353" windowHeight="4047" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1.2" sheetId="1" r:id="rId1"/>
+    <sheet name="1.4" sheetId="2" r:id="rId2"/>
+    <sheet name="1.8" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -84,16 +86,153 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>533866</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>108676</xdr:rowOff>
+      <xdr:colOff>562437</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>98595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40953402-B007-45C4-9738-0D3F0DAE5645}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="30161904" cy="15571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>495771</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>78466</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AC95C45-8C7F-4645-8A2D-D0AD56E962A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15836900"/>
+          <a:ext cx="30095238" cy="15733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>495771</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>107038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA419D3E-29EF-47D0-8A11-AC82D08ACBEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="31673800"/>
+          <a:ext cx="30095238" cy="15761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>505295</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>3357</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{706C5807-7AC6-4BE8-A223-B06203ED6DFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90716A8-BE25-4388-81E9-5FB5589C85BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -110,7 +249,320 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="30133333" cy="2657143"/>
+          <a:ext cx="30104762" cy="15476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>514818</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>164180</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A7DF1C-5FAB-4E7F-9413-A0BAA8A85C6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="19113500"/>
+          <a:ext cx="30114285" cy="15819047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>562437</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>49895</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0FC6F9-AC10-4138-9277-3916F812187A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="35678533"/>
+          <a:ext cx="30161904" cy="15704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114781</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>6281</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC2166D-5FF8-4B5C-8514-282C360FECEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="51515433"/>
+          <a:ext cx="4619048" cy="552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>524342</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>96433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6582B1-F91D-44FF-9764-91ECF6A97CAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="30123809" cy="15933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>524342</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>20243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48FC1A8-AC86-4712-8214-6332D2E7FB7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16018933"/>
+          <a:ext cx="30123809" cy="15857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>514818</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>164181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{231DD4CE-F5AA-4CA0-BE55-443E6EAFACAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="32037867"/>
+          <a:ext cx="30114285" cy="15819047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>524342</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>1957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11F2E49C-1F8C-461A-893A-3BCFE44BD458}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="48056800"/>
+          <a:ext cx="30123809" cy="1276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -421,7 +873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData/>
@@ -429,4 +883,34 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A284" sqref="A284"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="A265" sqref="A265"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>